<commit_message>
Upate for Instructors with CRUD for user and instructor always in web and API
</commit_message>
<xml_diff>
--- a/ملفات الاكسل لمشروع التخرج/instructors.xlsx
+++ b/ملفات الاكسل لمشروع التخرج/instructors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bit\Desktop\tamplete\final\timetable-pro\ملفات الاكسل لمشروع التخرج\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1219A4E-AA62-4FA2-B7C3-3BFBA172772E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A18548-AEB4-4AC1-A9C2-67BE8ABA9B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>department_id</t>
   </si>
   <si>
-    <t xml:space="preserve">م. رائد محمد مراد </t>
-  </si>
-  <si>
     <t>م. أكرم أبو جراد (ماجستير)</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>م. محمد أبو قاسم (بكالوريوس)</t>
   </si>
   <si>
-    <t>أ. إسماعيل دواس</t>
-  </si>
-  <si>
     <t>د. عز الدين عدوان (دكتوراه)</t>
   </si>
   <si>
@@ -93,22 +87,28 @@
     <t>أ. راجي تنيرة (بكالوريوس)</t>
   </si>
   <si>
-    <t xml:space="preserve">د. مراد أبومنسي </t>
-  </si>
-  <si>
     <t>أ. إلهام البحيصي (دبلوم)</t>
   </si>
   <si>
     <t>أ. علاء بشير (دبلوم)</t>
   </si>
   <si>
-    <t>د. محمد السردي</t>
-  </si>
-  <si>
-    <t xml:space="preserve">أ. عبد الله أبو قاسم </t>
-  </si>
-  <si>
     <t>م. عبد العزيز أبو الجبين (معيد)</t>
+  </si>
+  <si>
+    <t>م. رائد محمد مراد ( بكالوريوس )</t>
+  </si>
+  <si>
+    <t>أ. إسماعيل دواس ( بكالوريوس )</t>
+  </si>
+  <si>
+    <t>د. مراد أبومنسي ( بكالوريوس )</t>
+  </si>
+  <si>
+    <t>د. محمد السردي ( بكالوريوس )</t>
+  </si>
+  <si>
+    <t>أ. عبد الله أبو قاسم  ( بكالوريوس )</t>
   </si>
 </sst>
 </file>
@@ -439,14 +439,14 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.25" customWidth="1"/>
-    <col min="2" max="2" width="12.25" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="28.875" customWidth="1"/>
     <col min="4" max="4" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -472,7 +472,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -486,7 +486,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -500,7 +500,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -514,7 +514,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -528,7 +528,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -542,7 +542,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -556,7 +556,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -570,7 +570,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -584,7 +584,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -598,7 +598,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -612,7 +612,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -626,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -640,7 +640,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -654,7 +654,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -668,7 +668,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -682,7 +682,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -696,7 +696,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -710,7 +710,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -724,7 +724,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -738,7 +738,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -752,7 +752,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -766,7 +766,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -780,7 +780,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -794,7 +794,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D25">
         <v>1</v>

</xml_diff>

<commit_message>
Create and Update for Instructors with CRUD for instructor-section and instructor-subject always in web and API
</commit_message>
<xml_diff>
--- a/ملفات الاكسل لمشروع التخرج/instructors.xlsx
+++ b/ملفات الاكسل لمشروع التخرج/instructors.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bit\Desktop\tamplete\final\timetable-pro\ملفات الاكسل لمشروع التخرج\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A18548-AEB4-4AC1-A9C2-67BE8ABA9B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941C84B3-C7E3-423E-BA94-19381AB237B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>instructor_id</t>
   </si>
@@ -45,80 +45,172 @@
     <t>د. إياد أبو هدروس (دكتوراه)</t>
   </si>
   <si>
-    <t>أ. سفيان النزلي( دبلوم)</t>
-  </si>
-  <si>
     <t>م. إياد أبو سالم (بكالوريوس)</t>
   </si>
   <si>
     <t>م. محمد أبو حطب (ماجستير)</t>
   </si>
   <si>
-    <t>م. إيمان غيث (ماجستير)</t>
-  </si>
-  <si>
     <t>م. نيازي أبو حويج (ماجستير)</t>
   </si>
   <si>
-    <t>د. محمد النجار (دكتوراه)</t>
-  </si>
-  <si>
     <t>د. ناصر صباح (دكتوراه)</t>
   </si>
   <si>
-    <t>م. سعيد أبو الروس (ماجستير)</t>
-  </si>
-  <si>
     <t>م. أحمد العصار (ماجستير)</t>
   </si>
   <si>
-    <t>م. قصي فياض (بكالوريوس)</t>
-  </si>
-  <si>
     <t>م. محمد أبو قاسم (بكالوريوس)</t>
   </si>
   <si>
-    <t>د. عز الدين عدوان (دكتوراه)</t>
-  </si>
-  <si>
     <t>د. شوقي منصور (دكتوراه)</t>
   </si>
   <si>
-    <t>أ. راجي تنيرة (بكالوريوس)</t>
-  </si>
-  <si>
-    <t>أ. إلهام البحيصي (دبلوم)</t>
-  </si>
-  <si>
     <t>أ. علاء بشير (دبلوم)</t>
   </si>
   <si>
+    <t>د. محمد السردي</t>
+  </si>
+  <si>
     <t>م. عبد العزيز أبو الجبين (معيد)</t>
   </si>
   <si>
-    <t>م. رائد محمد مراد ( بكالوريوس )</t>
-  </si>
-  <si>
     <t>أ. إسماعيل دواس ( بكالوريوس )</t>
   </si>
   <si>
     <t>د. مراد أبومنسي ( بكالوريوس )</t>
   </si>
   <si>
-    <t>د. محمد السردي ( بكالوريوس )</t>
-  </si>
-  <si>
     <t>أ. عبد الله أبو قاسم  ( بكالوريوس )</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>raed55@gmail.com</t>
+  </si>
+  <si>
+    <t>eyad45@gmail.com</t>
+  </si>
+  <si>
+    <t>naser67@gmail.com</t>
+  </si>
+  <si>
+    <t>mohmed453@gmail.com</t>
+  </si>
+  <si>
+    <t>academic_degree</t>
+  </si>
+  <si>
+    <t>دبلوم</t>
+  </si>
+  <si>
+    <t>بكالوريوس</t>
+  </si>
+  <si>
+    <t>دكتوراه</t>
+  </si>
+  <si>
+    <t>معيد</t>
+  </si>
+  <si>
+    <t>ماجستير</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>PhD</t>
+  </si>
+  <si>
+    <t>دكتوراة</t>
+  </si>
+  <si>
+    <t>diploma</t>
+  </si>
+  <si>
+    <t>Bachelors</t>
+  </si>
+  <si>
+    <t>bachelor's</t>
+  </si>
+  <si>
+    <t>bachelors</t>
+  </si>
+  <si>
+    <t>م. رائد محمد مراد</t>
+  </si>
+  <si>
+    <t>أ. سفيان النزلي</t>
+  </si>
+  <si>
+    <t>م. إيمان غيث</t>
+  </si>
+  <si>
+    <t>د. محمد النجار</t>
+  </si>
+  <si>
+    <t>م. سعيد أبو الروس</t>
+  </si>
+  <si>
+    <t>م. قصي فياض</t>
+  </si>
+  <si>
+    <t>د. عز الدين عدوان</t>
+  </si>
+  <si>
+    <t>أ. راجي تنيرة</t>
+  </si>
+  <si>
+    <t>أ. إلهام البحيصي</t>
+  </si>
+  <si>
+    <t>م. مؤمن بسام صرصور (معيد)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">م. احمد مروان شعت </t>
+  </si>
+  <si>
+    <t>م. محسن عبد السلام الدردرلي</t>
+  </si>
+  <si>
+    <t>teacher</t>
+  </si>
+  <si>
+    <t>cse</t>
+  </si>
+  <si>
+    <t>CSE</t>
+  </si>
+  <si>
+    <t>ghghg22@gmail.com</t>
+  </si>
+  <si>
+    <t>max_weekly_hours</t>
+  </si>
+  <si>
+    <t>محست</t>
+  </si>
+  <si>
+    <t>بمكالوريوس</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,17 +239,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="ارتباط تشعبي" xfId="1" builtinId="8"/>
     <cellStyle name="عادي" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -436,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -447,10 +542,13 @@
     <col min="1" max="1" width="15.25" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="28.875" customWidth="1"/>
-    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +561,17 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -472,13 +579,22 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -491,8 +607,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -505,8 +624,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -514,13 +636,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -528,13 +656,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -542,13 +673,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -556,13 +690,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -570,13 +707,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -584,13 +724,19 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -598,13 +744,19 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -612,13 +764,19 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -626,13 +784,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -640,167 +801,272 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>15</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>21</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>23</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>23</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
+      <c r="C29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{11A64D80-E6C2-433E-A6A2-CFC86984418F}"/>
+    <hyperlink ref="E11" r:id="rId2" xr:uid="{EB38BC11-6215-41BC-887E-13850B75CE5C}"/>
+    <hyperlink ref="E18" r:id="rId3" xr:uid="{D805060A-6ACB-4222-A861-AABC08226897}"/>
+    <hyperlink ref="E15" r:id="rId4" xr:uid="{A82FE288-D818-49CF-A5FC-C73A3E8108E0}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{9EFCEC6A-0E7E-4011-A3EA-47D912BC1918}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Show final tables for each class, teacher and hall for the best chromosome from the algorithm
</commit_message>
<xml_diff>
--- a/ملفات الاكسل لمشروع التخرج/instructors.xlsx
+++ b/ملفات الاكسل لمشروع التخرج/instructors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bit\Desktop\tamplete\final\timetable-pro\ملفات الاكسل لمشروع التخرج\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941C84B3-C7E3-423E-BA94-19381AB237B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0569556-F4E1-4266-951B-790707898DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="163">
   <si>
     <t>instructor_id</t>
   </si>
@@ -111,9 +111,6 @@
     <t>دكتوراه</t>
   </si>
   <si>
-    <t>معيد</t>
-  </si>
-  <si>
     <t>ماجستير</t>
   </si>
   <si>
@@ -165,34 +162,358 @@
     <t>أ. إلهام البحيصي</t>
   </si>
   <si>
-    <t>م. مؤمن بسام صرصور (معيد)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">م. احمد مروان شعت </t>
-  </si>
-  <si>
-    <t>م. محسن عبد السلام الدردرلي</t>
-  </si>
-  <si>
-    <t>teacher</t>
-  </si>
-  <si>
-    <t>cse</t>
-  </si>
-  <si>
     <t>CSE</t>
   </si>
   <si>
-    <t>ghghg22@gmail.com</t>
-  </si>
-  <si>
     <t>max_weekly_hours</t>
   </si>
   <si>
-    <t>محست</t>
-  </si>
-  <si>
-    <t>بمكالوريوس</t>
+    <t xml:space="preserve">د. إبراهيم شاهين </t>
+  </si>
+  <si>
+    <t>أ. أديب زين الدين</t>
+  </si>
+  <si>
+    <t>أ. أرواح كرم</t>
+  </si>
+  <si>
+    <t>أ. إحسان أبو عمرة</t>
+  </si>
+  <si>
+    <t>أ. أحمد أبو مغصيب</t>
+  </si>
+  <si>
+    <t>أحمد الأغا</t>
+  </si>
+  <si>
+    <t>أحمد شبير</t>
+  </si>
+  <si>
+    <t>أ. أحمد العديني</t>
+  </si>
+  <si>
+    <t>أسامة زهري</t>
+  </si>
+  <si>
+    <t>أ. أكرم جرادة</t>
+  </si>
+  <si>
+    <t>أكرم مطر</t>
+  </si>
+  <si>
+    <t>أمل العجرمي</t>
+  </si>
+  <si>
+    <t>آمنة أبو خشيبة</t>
+  </si>
+  <si>
+    <t>آمال الحيلة</t>
+  </si>
+  <si>
+    <t>إياد المغاري</t>
+  </si>
+  <si>
+    <t>إياد القرا</t>
+  </si>
+  <si>
+    <t>أيمن الدنف</t>
+  </si>
+  <si>
+    <t>أيمن نوفل</t>
+  </si>
+  <si>
+    <t>أيمن تنيرة</t>
+  </si>
+  <si>
+    <t>بدران عوض</t>
+  </si>
+  <si>
+    <t>تحسين العبادلة</t>
+  </si>
+  <si>
+    <t>أ. جيهان صرصور</t>
+  </si>
+  <si>
+    <t>حسام أبو شاويش</t>
+  </si>
+  <si>
+    <t>حسن أبو عمرة</t>
+  </si>
+  <si>
+    <t>خالد أبو قوطة</t>
+  </si>
+  <si>
+    <t>د. خليل جبر</t>
+  </si>
+  <si>
+    <t>دولت أبو معيلق</t>
+  </si>
+  <si>
+    <t>راجي تنيرة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">أ. رمزي غنيم </t>
+  </si>
+  <si>
+    <t xml:space="preserve">رياض عياد </t>
+  </si>
+  <si>
+    <t>د. زياد أبو حليب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سامي سلامة </t>
+  </si>
+  <si>
+    <t xml:space="preserve">سمير حلس </t>
+  </si>
+  <si>
+    <t>سهير حرب</t>
+  </si>
+  <si>
+    <t>شذا أبو سليم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">صبحي عبد القادر </t>
+  </si>
+  <si>
+    <t>عاطف الشويخ</t>
+  </si>
+  <si>
+    <t>عائشة الكرد</t>
+  </si>
+  <si>
+    <t>عبد القادر مسلم</t>
+  </si>
+  <si>
+    <t>عبد الرحيم السحار</t>
+  </si>
+  <si>
+    <t xml:space="preserve">أ. عبد المنعم نجم </t>
+  </si>
+  <si>
+    <t xml:space="preserve">د. عبد الحفيظ العيلة </t>
+  </si>
+  <si>
+    <t>أ. علاء مزيد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">غسان الدلو </t>
+  </si>
+  <si>
+    <t>أ. غسان صباح</t>
+  </si>
+  <si>
+    <t>فاتن أبو شمالة</t>
+  </si>
+  <si>
+    <t>م. فؤاد أبو عويمر</t>
+  </si>
+  <si>
+    <t>كمال نوفل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">أ. لبنى الأستاذ </t>
+  </si>
+  <si>
+    <t>مؤنس الحنجوري</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ماهر حمادة </t>
+  </si>
+  <si>
+    <t>د. محمد البحيصي</t>
+  </si>
+  <si>
+    <t>محمد النجار</t>
+  </si>
+  <si>
+    <t>أ. محمد جحيش</t>
+  </si>
+  <si>
+    <t>محمد تنيرة</t>
+  </si>
+  <si>
+    <t>محمد المصري</t>
+  </si>
+  <si>
+    <t>أ. محمد الدربي</t>
+  </si>
+  <si>
+    <t>محمد مرتجى</t>
+  </si>
+  <si>
+    <t>د. مروان جلمبو</t>
+  </si>
+  <si>
+    <t>منال حجازي</t>
+  </si>
+  <si>
+    <t>د. منتصر حجازي</t>
+  </si>
+  <si>
+    <t>د. منصور الأيوبي</t>
+  </si>
+  <si>
+    <t>ميادة مغاري</t>
+  </si>
+  <si>
+    <t>أ. نادية صافي</t>
+  </si>
+  <si>
+    <t>ناهض أبو شقة</t>
+  </si>
+  <si>
+    <t>أ. نايفة ذيبة</t>
+  </si>
+  <si>
+    <t>نسرين مخيمر</t>
+  </si>
+  <si>
+    <t>أ. نسيم زقوت</t>
+  </si>
+  <si>
+    <t>نعيم المصري</t>
+  </si>
+  <si>
+    <t>نهاد حماد</t>
+  </si>
+  <si>
+    <t>نيازي أبو حويج</t>
+  </si>
+  <si>
+    <t>هادي النبريص</t>
+  </si>
+  <si>
+    <t>هاني عبد الباري</t>
+  </si>
+  <si>
+    <t>هاني السويركي</t>
+  </si>
+  <si>
+    <t>هبة أبو عرب</t>
+  </si>
+  <si>
+    <t>هيثم عياش</t>
+  </si>
+  <si>
+    <t>ياسر رضوان</t>
+  </si>
+  <si>
+    <t>أ. ياسر برهوم</t>
+  </si>
+  <si>
+    <t>أ. ياسر أبو لوز</t>
+  </si>
+  <si>
+    <t>يوسف منصور</t>
+  </si>
+  <si>
+    <t>أ. أيمن الشيخ عيد</t>
+  </si>
+  <si>
+    <t>إبراهيم أبو صالح</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رامي الزقزوق </t>
+  </si>
+  <si>
+    <t>أ. شادي الدلو</t>
+  </si>
+  <si>
+    <t>عبد الهادي التلباني</t>
+  </si>
+  <si>
+    <t>هالة أبو شاويش</t>
+  </si>
+  <si>
+    <t>د. راوية أبو الخير</t>
+  </si>
+  <si>
+    <t>هاني حجازي</t>
+  </si>
+  <si>
+    <t>رائده أبو حجر</t>
+  </si>
+  <si>
+    <t>أ. محمد أبو عمرة</t>
+  </si>
+  <si>
+    <t>صلاح قاسم</t>
+  </si>
+  <si>
+    <t>أ. محمد شعبان</t>
+  </si>
+  <si>
+    <t>أ. محمد درويش</t>
+  </si>
+  <si>
+    <t>أ. معين سلمان</t>
+  </si>
+  <si>
+    <t>أ. سعاد كلوب</t>
+  </si>
+  <si>
+    <t>يوسف القرماني</t>
+  </si>
+  <si>
+    <t>م. أمجد أبو الجديان</t>
+  </si>
+  <si>
+    <t>محمد الطبجي</t>
+  </si>
+  <si>
+    <t xml:space="preserve">محمد لبد </t>
+  </si>
+  <si>
+    <t>أ. ضياء أبو سلطان</t>
+  </si>
+  <si>
+    <t>م. رانيه الهببيل</t>
+  </si>
+  <si>
+    <t>إسراء سمارة</t>
+  </si>
+  <si>
+    <t>كرم النيرب</t>
+  </si>
+  <si>
+    <t>هبة أبو عجمي</t>
+  </si>
+  <si>
+    <t>م. محمد صالحة</t>
+  </si>
+  <si>
+    <t>أ. عزيزه مصبح</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رائد أحمد </t>
+  </si>
+  <si>
+    <t xml:space="preserve">بسمة أبو صبحة </t>
+  </si>
+  <si>
+    <t>إيمان الزعانين</t>
+  </si>
+  <si>
+    <t>أ. لؤي قنن</t>
+  </si>
+  <si>
+    <t>محمد دحلان</t>
+  </si>
+  <si>
+    <t>عبد الرحمن خواص</t>
+  </si>
+  <si>
+    <t>تسنيم الششنية</t>
+  </si>
+  <si>
+    <t>هاني عياش</t>
+  </si>
+  <si>
+    <t>حليمة النعامي</t>
+  </si>
+  <si>
+    <t>دعاء لبد</t>
   </si>
 </sst>
 </file>
@@ -531,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="B119" workbookViewId="0">
+      <selection activeCell="F142" sqref="F142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -568,7 +889,7 @@
         <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -579,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -588,10 +909,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -608,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -627,6 +948,9 @@
       <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="G4">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -636,16 +960,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -662,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -676,10 +1000,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -690,13 +1014,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G8">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -713,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -724,16 +1051,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -753,7 +1080,10 @@
         <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="G11">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -764,16 +1094,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -787,10 +1117,10 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -801,7 +1131,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -809,263 +1139,2190 @@
       <c r="F14" t="s">
         <v>26</v>
       </c>
+      <c r="G14">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15">
         <v>25</v>
-      </c>
-      <c r="B15">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15">
-        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="F16" t="s">
-        <v>28</v>
-      </c>
       <c r="G16">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
       <c r="G17">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="G18">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="F20" t="s">
-        <v>27</v>
-      </c>
       <c r="G20">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21">
+        <v>23</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>18</v>
-      </c>
-      <c r="C22" t="s">
-        <v>44</v>
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="F22" t="s">
-        <v>36</v>
+      <c r="G22">
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23">
+        <v>23</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>20</v>
-      </c>
-      <c r="C24" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="F24" t="s">
-        <v>25</v>
+      <c r="G24">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>21</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
+      <c r="G25">
+        <v>23</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>22</v>
-      </c>
       <c r="B26">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
       </c>
       <c r="F26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>23</v>
-      </c>
-      <c r="B27">
-        <v>23</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>24</v>
-      </c>
-      <c r="B28">
-        <v>24</v>
-      </c>
-      <c r="C28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>23</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>42</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>45</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+      <c r="G44">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+      <c r="G45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>47</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+      <c r="G46">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>48</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+      <c r="G47">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <v>49</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+      <c r="G48">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>51</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>52</v>
+      </c>
+      <c r="C51" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" t="s">
+        <v>27</v>
+      </c>
+      <c r="G51">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B52">
+        <v>53</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B53">
         <v>54</v>
       </c>
-      <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="C53" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" t="s">
+        <v>45</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+      <c r="G53">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B54">
         <v>55</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" t="s">
+        <v>45</v>
+      </c>
+      <c r="F54" t="s">
+        <v>26</v>
+      </c>
+      <c r="G54">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>56</v>
+      </c>
+      <c r="C55" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" t="s">
+        <v>45</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+      <c r="G55">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>57</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" t="s">
+        <v>27</v>
+      </c>
+      <c r="G56">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" t="s">
+        <v>45</v>
+      </c>
+      <c r="F57" t="s">
+        <v>27</v>
+      </c>
+      <c r="G57">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>59</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D58" t="s">
+        <v>45</v>
+      </c>
+      <c r="F58" t="s">
+        <v>26</v>
+      </c>
+      <c r="G58">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>60</v>
+      </c>
+      <c r="C59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" t="s">
+        <v>28</v>
+      </c>
+      <c r="G59">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>61</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60" t="s">
+        <v>45</v>
+      </c>
+      <c r="F60" t="s">
+        <v>26</v>
+      </c>
+      <c r="G60">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>62</v>
+      </c>
+      <c r="C61" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" t="s">
+        <v>45</v>
+      </c>
+      <c r="F61" t="s">
+        <v>26</v>
+      </c>
+      <c r="G61">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>63</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D62" t="s">
+        <v>45</v>
+      </c>
+      <c r="F62" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>64</v>
+      </c>
+      <c r="C63" t="s">
+        <v>84</v>
+      </c>
+      <c r="D63" t="s">
+        <v>45</v>
+      </c>
+      <c r="F63" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>65</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D64" t="s">
+        <v>45</v>
+      </c>
+      <c r="F64" t="s">
+        <v>26</v>
+      </c>
+      <c r="G64">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>66</v>
+      </c>
+      <c r="C65" t="s">
+        <v>86</v>
+      </c>
+      <c r="D65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F65" t="s">
+        <v>26</v>
+      </c>
+      <c r="G65">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>67</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" t="s">
+        <v>45</v>
+      </c>
+      <c r="F66" t="s">
+        <v>26</v>
+      </c>
+      <c r="G66">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>68</v>
+      </c>
+      <c r="C67" t="s">
+        <v>88</v>
+      </c>
+      <c r="D67" t="s">
+        <v>45</v>
+      </c>
+      <c r="F67" t="s">
+        <v>27</v>
+      </c>
+      <c r="G67">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>69</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D68" t="s">
+        <v>45</v>
+      </c>
+      <c r="F68" t="s">
+        <v>26</v>
+      </c>
+      <c r="G68">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>70</v>
+      </c>
+      <c r="C69" t="s">
+        <v>90</v>
+      </c>
+      <c r="D69" t="s">
+        <v>45</v>
+      </c>
+      <c r="F69" t="s">
+        <v>26</v>
+      </c>
+      <c r="G69">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>71</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D70" t="s">
+        <v>45</v>
+      </c>
+      <c r="F70" t="s">
+        <v>26</v>
+      </c>
+      <c r="G70">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>72</v>
+      </c>
+      <c r="C71" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" t="s">
+        <v>45</v>
+      </c>
+      <c r="F71" t="s">
+        <v>26</v>
+      </c>
+      <c r="G71">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>73</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72" t="s">
+        <v>45</v>
+      </c>
+      <c r="F72" t="s">
+        <v>26</v>
+      </c>
+      <c r="G72">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>74</v>
+      </c>
+      <c r="C73" t="s">
+        <v>94</v>
+      </c>
+      <c r="D73" t="s">
+        <v>45</v>
+      </c>
+      <c r="F73" t="s">
+        <v>26</v>
+      </c>
+      <c r="G73">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>75</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D74" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" t="s">
+        <v>26</v>
+      </c>
+      <c r="G74">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B75">
+        <v>76</v>
+      </c>
+      <c r="C75" t="s">
+        <v>96</v>
+      </c>
+      <c r="D75" t="s">
+        <v>45</v>
+      </c>
+      <c r="F75" t="s">
+        <v>26</v>
+      </c>
+      <c r="G75">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>77</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D76" t="s">
+        <v>45</v>
+      </c>
+      <c r="F76" t="s">
+        <v>27</v>
+      </c>
+      <c r="G76">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>78</v>
+      </c>
+      <c r="C77" t="s">
+        <v>98</v>
+      </c>
+      <c r="D77" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" t="s">
+        <v>27</v>
+      </c>
+      <c r="G77">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>79</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D78" t="s">
+        <v>45</v>
+      </c>
+      <c r="F78" t="s">
+        <v>26</v>
+      </c>
+      <c r="G78">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>80</v>
+      </c>
+      <c r="C79" t="s">
+        <v>100</v>
+      </c>
+      <c r="D79" t="s">
+        <v>45</v>
+      </c>
+      <c r="F79" t="s">
+        <v>26</v>
+      </c>
+      <c r="G79">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>81</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D80" t="s">
+        <v>45</v>
+      </c>
+      <c r="F80" t="s">
+        <v>26</v>
+      </c>
+      <c r="G80">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>82</v>
+      </c>
+      <c r="C81" t="s">
+        <v>102</v>
+      </c>
+      <c r="D81" t="s">
+        <v>45</v>
+      </c>
+      <c r="F81" t="s">
+        <v>26</v>
+      </c>
+      <c r="G81">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>83</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D82" t="s">
+        <v>45</v>
+      </c>
+      <c r="F82" t="s">
+        <v>26</v>
+      </c>
+      <c r="G82">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>84</v>
+      </c>
+      <c r="C83" t="s">
+        <v>104</v>
+      </c>
+      <c r="D83" t="s">
+        <v>45</v>
+      </c>
+      <c r="F83" t="s">
+        <v>26</v>
+      </c>
+      <c r="G83">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>85</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D84" t="s">
+        <v>45</v>
+      </c>
+      <c r="F84" t="s">
+        <v>27</v>
+      </c>
+      <c r="G84">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>86</v>
+      </c>
+      <c r="C85" t="s">
+        <v>106</v>
+      </c>
+      <c r="D85" t="s">
+        <v>45</v>
+      </c>
+      <c r="F85" t="s">
+        <v>26</v>
+      </c>
+      <c r="G85">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>87</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D86" t="s">
+        <v>45</v>
+      </c>
+      <c r="F86" t="s">
+        <v>27</v>
+      </c>
+      <c r="G86">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>88</v>
+      </c>
+      <c r="C87" t="s">
+        <v>108</v>
+      </c>
+      <c r="D87" t="s">
+        <v>45</v>
+      </c>
+      <c r="F87" t="s">
+        <v>27</v>
+      </c>
+      <c r="G87">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>89</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D88" t="s">
+        <v>45</v>
+      </c>
+      <c r="F88" t="s">
+        <v>28</v>
+      </c>
+      <c r="G88">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>90</v>
+      </c>
+      <c r="C89" t="s">
+        <v>110</v>
+      </c>
+      <c r="D89" t="s">
+        <v>45</v>
+      </c>
+      <c r="F89" t="s">
+        <v>26</v>
+      </c>
+      <c r="G89">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>91</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D90" t="s">
+        <v>45</v>
+      </c>
+      <c r="F90" t="s">
+        <v>26</v>
+      </c>
+      <c r="G90">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>92</v>
+      </c>
+      <c r="C91" t="s">
+        <v>112</v>
+      </c>
+      <c r="D91" t="s">
+        <v>45</v>
+      </c>
+      <c r="F91" t="s">
+        <v>26</v>
+      </c>
+      <c r="G91">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>93</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D92" t="s">
+        <v>45</v>
+      </c>
+      <c r="F92" t="s">
+        <v>26</v>
+      </c>
+      <c r="G92">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>94</v>
+      </c>
+      <c r="C93" t="s">
+        <v>114</v>
+      </c>
+      <c r="D93" t="s">
+        <v>45</v>
+      </c>
+      <c r="F93" t="s">
+        <v>26</v>
+      </c>
+      <c r="G93">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>95</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D94" t="s">
+        <v>45</v>
+      </c>
+      <c r="F94" t="s">
+        <v>26</v>
+      </c>
+      <c r="G94">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>96</v>
+      </c>
+      <c r="C95" t="s">
+        <v>116</v>
+      </c>
+      <c r="D95" t="s">
+        <v>45</v>
+      </c>
+      <c r="F95" t="s">
+        <v>26</v>
+      </c>
+      <c r="G95">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B96">
+        <v>97</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D96" t="s">
+        <v>45</v>
+      </c>
+      <c r="F96" t="s">
+        <v>26</v>
+      </c>
+      <c r="G96">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>98</v>
+      </c>
+      <c r="C97" t="s">
+        <v>118</v>
+      </c>
+      <c r="D97" t="s">
+        <v>45</v>
+      </c>
+      <c r="F97" t="s">
+        <v>26</v>
+      </c>
+      <c r="G97">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B98">
+        <v>99</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D98" t="s">
+        <v>45</v>
+      </c>
+      <c r="F98" t="s">
+        <v>26</v>
+      </c>
+      <c r="G98">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B99">
+        <v>100</v>
+      </c>
+      <c r="C99" t="s">
+        <v>120</v>
+      </c>
+      <c r="D99" t="s">
+        <v>45</v>
+      </c>
+      <c r="F99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G99">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>101</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D100" t="s">
+        <v>45</v>
+      </c>
+      <c r="F100" t="s">
+        <v>26</v>
+      </c>
+      <c r="G100">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>102</v>
+      </c>
+      <c r="C101" t="s">
+        <v>122</v>
+      </c>
+      <c r="D101" t="s">
+        <v>45</v>
+      </c>
+      <c r="F101" t="s">
+        <v>26</v>
+      </c>
+      <c r="G101">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>103</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D102" t="s">
+        <v>45</v>
+      </c>
+      <c r="F102" t="s">
+        <v>26</v>
+      </c>
+      <c r="G102">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B103">
+        <v>104</v>
+      </c>
+      <c r="C103" t="s">
+        <v>124</v>
+      </c>
+      <c r="D103" t="s">
+        <v>45</v>
+      </c>
+      <c r="F103" t="s">
+        <v>26</v>
+      </c>
+      <c r="G103">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>105</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D104" t="s">
+        <v>45</v>
+      </c>
+      <c r="F104" t="s">
+        <v>26</v>
+      </c>
+      <c r="G104">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>106</v>
+      </c>
+      <c r="C105" t="s">
+        <v>126</v>
+      </c>
+      <c r="D105" t="s">
+        <v>45</v>
+      </c>
+      <c r="F105" t="s">
+        <v>26</v>
+      </c>
+      <c r="G105">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>107</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D106" t="s">
+        <v>45</v>
+      </c>
+      <c r="F106" t="s">
+        <v>26</v>
+      </c>
+      <c r="G106">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>108</v>
+      </c>
+      <c r="C107" t="s">
+        <v>128</v>
+      </c>
+      <c r="D107" t="s">
+        <v>45</v>
+      </c>
+      <c r="F107" t="s">
+        <v>26</v>
+      </c>
+      <c r="G107">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>109</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D108" t="s">
+        <v>45</v>
+      </c>
+      <c r="F108" t="s">
+        <v>26</v>
+      </c>
+      <c r="G108">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>110</v>
+      </c>
+      <c r="C109" t="s">
+        <v>130</v>
+      </c>
+      <c r="D109" t="s">
+        <v>45</v>
+      </c>
+      <c r="F109" t="s">
+        <v>26</v>
+      </c>
+      <c r="G109">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>111</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D110" t="s">
+        <v>45</v>
+      </c>
+      <c r="F110" t="s">
+        <v>26</v>
+      </c>
+      <c r="G110">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B111">
+        <v>112</v>
+      </c>
+      <c r="C111" t="s">
+        <v>132</v>
+      </c>
+      <c r="D111" t="s">
+        <v>45</v>
+      </c>
+      <c r="F111" t="s">
+        <v>26</v>
+      </c>
+      <c r="G111">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>113</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D112" t="s">
+        <v>45</v>
+      </c>
+      <c r="F112" t="s">
+        <v>27</v>
+      </c>
+      <c r="G112">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B113">
+        <v>114</v>
+      </c>
+      <c r="C113" t="s">
+        <v>134</v>
+      </c>
+      <c r="D113" t="s">
+        <v>45</v>
+      </c>
+      <c r="F113" t="s">
+        <v>26</v>
+      </c>
+      <c r="G113">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>115</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D114" t="s">
+        <v>45</v>
+      </c>
+      <c r="F114" t="s">
+        <v>26</v>
+      </c>
+      <c r="G114">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B115">
+        <v>116</v>
+      </c>
+      <c r="C115" t="s">
+        <v>136</v>
+      </c>
+      <c r="D115" t="s">
+        <v>45</v>
+      </c>
+      <c r="F115" t="s">
+        <v>26</v>
+      </c>
+      <c r="G115">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B116">
+        <v>117</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D116" t="s">
+        <v>45</v>
+      </c>
+      <c r="F116" t="s">
+        <v>26</v>
+      </c>
+      <c r="G116">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>118</v>
+      </c>
+      <c r="C117" t="s">
+        <v>138</v>
+      </c>
+      <c r="D117" t="s">
+        <v>45</v>
+      </c>
+      <c r="F117" t="s">
+        <v>26</v>
+      </c>
+      <c r="G117">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>119</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D118" t="s">
+        <v>45</v>
+      </c>
+      <c r="F118" t="s">
+        <v>26</v>
+      </c>
+      <c r="G118">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>120</v>
+      </c>
+      <c r="C119" t="s">
+        <v>140</v>
+      </c>
+      <c r="D119" t="s">
+        <v>45</v>
+      </c>
+      <c r="F119" t="s">
+        <v>26</v>
+      </c>
+      <c r="G119">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B120">
+        <v>121</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D120" t="s">
+        <v>45</v>
+      </c>
+      <c r="F120" t="s">
+        <v>26</v>
+      </c>
+      <c r="G120">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>122</v>
+      </c>
+      <c r="C121" t="s">
+        <v>142</v>
+      </c>
+      <c r="D121" t="s">
+        <v>45</v>
+      </c>
+      <c r="F121" t="s">
+        <v>26</v>
+      </c>
+      <c r="G121">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B122">
+        <v>123</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D122" t="s">
+        <v>45</v>
+      </c>
+      <c r="F122" t="s">
+        <v>26</v>
+      </c>
+      <c r="G122">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B123">
+        <v>124</v>
+      </c>
+      <c r="C123" t="s">
+        <v>144</v>
+      </c>
+      <c r="D123" t="s">
+        <v>45</v>
+      </c>
+      <c r="F123" t="s">
+        <v>26</v>
+      </c>
+      <c r="G123">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B124">
+        <v>125</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D124" t="s">
+        <v>45</v>
+      </c>
+      <c r="F124" t="s">
+        <v>26</v>
+      </c>
+      <c r="G124">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B125">
+        <v>126</v>
+      </c>
+      <c r="C125" t="s">
+        <v>146</v>
+      </c>
+      <c r="D125" t="s">
+        <v>45</v>
+      </c>
+      <c r="F125" t="s">
+        <v>26</v>
+      </c>
+      <c r="G125">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B126">
+        <v>127</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D126" t="s">
+        <v>45</v>
+      </c>
+      <c r="F126" t="s">
+        <v>26</v>
+      </c>
+      <c r="G126">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B127">
+        <v>128</v>
+      </c>
+      <c r="C127" t="s">
+        <v>148</v>
+      </c>
+      <c r="D127" t="s">
+        <v>45</v>
+      </c>
+      <c r="F127" t="s">
+        <v>26</v>
+      </c>
+      <c r="G127">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B128">
+        <v>129</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D128" t="s">
+        <v>45</v>
+      </c>
+      <c r="F128" t="s">
+        <v>26</v>
+      </c>
+      <c r="G128">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B129">
+        <v>130</v>
+      </c>
+      <c r="C129" t="s">
+        <v>150</v>
+      </c>
+      <c r="D129" t="s">
+        <v>45</v>
+      </c>
+      <c r="F129" t="s">
+        <v>26</v>
+      </c>
+      <c r="G129">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B130">
+        <v>131</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D130" t="s">
+        <v>45</v>
+      </c>
+      <c r="F130" t="s">
+        <v>26</v>
+      </c>
+      <c r="G130">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>132</v>
+      </c>
+      <c r="C131" t="s">
+        <v>152</v>
+      </c>
+      <c r="D131" t="s">
+        <v>45</v>
+      </c>
+      <c r="F131" t="s">
+        <v>26</v>
+      </c>
+      <c r="G131">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B132">
+        <v>133</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D132" t="s">
+        <v>45</v>
+      </c>
+      <c r="F132" t="s">
+        <v>26</v>
+      </c>
+      <c r="G132">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B133">
+        <v>134</v>
+      </c>
+      <c r="C133" t="s">
+        <v>154</v>
+      </c>
+      <c r="D133" t="s">
+        <v>45</v>
+      </c>
+      <c r="F133" t="s">
+        <v>26</v>
+      </c>
+      <c r="G133">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B134">
+        <v>135</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D134" t="s">
+        <v>45</v>
+      </c>
+      <c r="F134" t="s">
+        <v>26</v>
+      </c>
+      <c r="G134">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B135">
+        <v>136</v>
+      </c>
+      <c r="C135" t="s">
+        <v>156</v>
+      </c>
+      <c r="D135" t="s">
+        <v>45</v>
+      </c>
+      <c r="F135" t="s">
+        <v>26</v>
+      </c>
+      <c r="G135">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B136">
+        <v>137</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D136" t="s">
+        <v>45</v>
+      </c>
+      <c r="F136" t="s">
+        <v>26</v>
+      </c>
+      <c r="G136">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B137">
+        <v>138</v>
+      </c>
+      <c r="C137" t="s">
+        <v>158</v>
+      </c>
+      <c r="D137" t="s">
+        <v>45</v>
+      </c>
+      <c r="F137" t="s">
+        <v>26</v>
+      </c>
+      <c r="G137">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B138">
+        <v>139</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D138" t="s">
+        <v>45</v>
+      </c>
+      <c r="F138" t="s">
+        <v>26</v>
+      </c>
+      <c r="G138">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B139">
+        <v>140</v>
+      </c>
+      <c r="C139" t="s">
+        <v>160</v>
+      </c>
+      <c r="D139" t="s">
+        <v>45</v>
+      </c>
+      <c r="F139" t="s">
+        <v>26</v>
+      </c>
+      <c r="G139">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B140">
+        <v>141</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D140" t="s">
+        <v>45</v>
+      </c>
+      <c r="F140" t="s">
+        <v>26</v>
+      </c>
+      <c r="G140">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B141">
+        <v>142</v>
+      </c>
+      <c r="C141" t="s">
+        <v>162</v>
+      </c>
+      <c r="D141" t="s">
+        <v>45</v>
+      </c>
+      <c r="F141" t="s">
+        <v>26</v>
+      </c>
+      <c r="G141">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{11A64D80-E6C2-433E-A6A2-CFC86984418F}"/>
     <hyperlink ref="E11" r:id="rId2" xr:uid="{EB38BC11-6215-41BC-887E-13850B75CE5C}"/>
-    <hyperlink ref="E18" r:id="rId3" xr:uid="{D805060A-6ACB-4222-A861-AABC08226897}"/>
-    <hyperlink ref="E15" r:id="rId4" xr:uid="{A82FE288-D818-49CF-A5FC-C73A3E8108E0}"/>
-    <hyperlink ref="E2" r:id="rId5" xr:uid="{9EFCEC6A-0E7E-4011-A3EA-47D912BC1918}"/>
+    <hyperlink ref="E15" r:id="rId3" xr:uid="{D805060A-6ACB-4222-A861-AABC08226897}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{9EFCEC6A-0E7E-4011-A3EA-47D912BC1918}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>